<commit_message>
slight changes in the plot function
</commit_message>
<xml_diff>
--- a/inputs/input_data.xlsx
+++ b/inputs/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sayadi\Documents\myGitHub\offgridders\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B402B7BB-4E63-4F51-A6F6-CFD3F9C13ECB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00253A26-447E-4736-859B-6BC05CF50359}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -1598,6 +1598,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1612,9 +1615,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2206,8 +2206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A43" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2661,8 +2661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3735,8 +3735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3863,10 +3863,10 @@
         <v>0</v>
       </c>
       <c r="C11" s="18">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D11" s="18">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -3892,7 +3892,7 @@
   <dimension ref="A1:AMI15"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4133,16 +4133,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4157,8 +4157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AMD38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D38"/>
+    <sheetView topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4333,7 +4333,7 @@
         <v>268</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C18" s="36" t="s">
         <v>39</v>
@@ -4808,29 +4808,29 @@
       <c r="A4" s="32" t="s">
         <v>291</v>
       </c>
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="69" t="s">
         <v>292</v>
       </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>293</v>
       </c>
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="69" t="s">
         <v>294</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
     </row>
     <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="40" t="s">
@@ -4915,12 +4915,12 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E16" s="71" t="s">
+      <c r="E16" s="72" t="s">
         <v>307</v>
       </c>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71"/>
-      <c r="H16" s="71"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="72"/>
+      <c r="H16" s="72"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="45" t="s">
@@ -4952,7 +4952,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="72" t="s">
+      <c r="A18" s="73" t="s">
         <v>314</v>
       </c>
       <c r="B18" s="48" t="s">
@@ -4973,7 +4973,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="72"/>
+      <c r="A19" s="73"/>
       <c r="B19" s="53" t="s">
         <v>317</v>
       </c>
@@ -4992,7 +4992,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="72" t="s">
+      <c r="A20" s="73" t="s">
         <v>319</v>
       </c>
       <c r="B20" s="48" t="s">
@@ -5013,7 +5013,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="72"/>
+      <c r="A21" s="73"/>
       <c r="B21" s="57" t="s">
         <v>322</v>
       </c>
@@ -5032,7 +5032,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="72"/>
+      <c r="A22" s="73"/>
       <c r="B22" s="57" t="s">
         <v>324</v>
       </c>
@@ -5059,7 +5059,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="72"/>
+      <c r="A23" s="73"/>
       <c r="B23" s="53" t="s">
         <v>326</v>
       </c>
@@ -5086,7 +5086,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="73" t="s">
+      <c r="A24" s="74" t="s">
         <v>328</v>
       </c>
       <c r="B24" s="61" t="s">
@@ -5113,10 +5113,10 @@
       <c r="I24" s="56" t="b">
         <v>1</v>
       </c>
-      <c r="N24" s="69"/>
+      <c r="N24" s="70"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="73"/>
+      <c r="A25" s="74"/>
       <c r="B25" s="61" t="s">
         <v>331</v>
       </c>
@@ -5133,10 +5133,10 @@
       <c r="I25" s="56" t="b">
         <v>0</v>
       </c>
-      <c r="N25" s="69"/>
+      <c r="N25" s="70"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="73"/>
+      <c r="A26" s="74"/>
       <c r="B26" s="62" t="s">
         <v>333</v>
       </c>
@@ -5161,10 +5161,10 @@
       <c r="I26" s="56" t="b">
         <v>1</v>
       </c>
-      <c r="N26" s="69"/>
+      <c r="N26" s="70"/>
     </row>
     <row r="27" spans="1:14" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="70" t="s">
+      <c r="A27" s="71" t="s">
         <v>335</v>
       </c>
       <c r="B27" s="63" t="s">
@@ -5196,7 +5196,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="70"/>
+      <c r="A28" s="71"/>
       <c r="B28" s="61" t="s">
         <v>339</v>
       </c>
@@ -5223,7 +5223,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="70"/>
+      <c r="A29" s="71"/>
       <c r="B29" s="62" t="s">
         <v>341</v>
       </c>
@@ -5257,10 +5257,10 @@
       <c r="H30" s="9"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="71" t="s">
+      <c r="A32" s="72" t="s">
         <v>299</v>
       </c>
-      <c r="B32" s="71"/>
+      <c r="B32" s="72"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="44" t="s">
@@ -5292,11 +5292,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B7:H7"/>
     <mergeCell ref="N24:N26"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="A32:B32"/>
@@ -5305,6 +5300,11 @@
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A20:A23"/>
     <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>